<commit_message>
URL Type Description Type
</commit_message>
<xml_diff>
--- a/admin/rdm/Digiplois_RDM_not_ObjK.xlsx
+++ b/admin/rdm/Digiplois_RDM_not_ObjK.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tw/PycharmProjects/arches/digipolis-arches-pkg/admin/rdm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sa83755\Documents\LH\digipolis-arches-pkg\admin\rdm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D347AC9-53D8-4244-A3FE-F28F9CDED94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{5FA84475-12ED-5642-BEC8-9D4C34E74F64}"/>
+    <workbookView xWindow="1176" yWindow="1464" windowWidth="27240" windowHeight="16044" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Correspondence Type" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
   <definedNames>
     <definedName name="date_types" localSheetId="2">'Date Type'!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,9 +49,9 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{A055A257-188C-384D-8C2C-31FF8B9C0633}" name="date_types" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/tw/PycharmProjects/arches/digipolis_importer/import/csv/lookup/date_types.csv" decimal="," thousands=" " tab="0" comma="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="date_types" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr sourceFile="/Users/tw/PycharmProjects/arches/digipolis_importer/import/csv/lookup/date_types.csv" decimal="," thousands=" " tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -63,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="135">
   <si>
     <t>code</t>
   </si>
@@ -77,9 +76,6 @@
     <t>Verzender</t>
   </si>
   <si>
-    <t>new_concept</t>
-  </si>
-  <si>
     <t>AS IS!</t>
   </si>
   <si>
@@ -257,9 +253,6 @@
     <t>LEAVE AS IS UNTIL WE HAVE IIIF LINKS OR NEW DEPOT LINKS AND TYPES</t>
   </si>
   <si>
-    <t>Concept</t>
-  </si>
-  <si>
     <t>Canvas</t>
   </si>
   <si>
@@ -272,9 +265,6 @@
     <t>Sheet</t>
   </si>
   <si>
-    <t>new_concepts</t>
-  </si>
-  <si>
     <t>(not used, here as examples. Add likely ones)</t>
   </si>
   <si>
@@ -378,12 +368,111 @@
   </si>
   <si>
     <t>Merge w beschrijvning, annotatie ??</t>
+  </si>
+  <si>
+    <t>thesaurus</t>
+  </si>
+  <si>
+    <t>new concept</t>
+  </si>
+  <si>
+    <t>AAT ID</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Beschrijving Type\</t>
+  </si>
+  <si>
+    <t>descriptive note</t>
+  </si>
+  <si>
+    <t>detailbeschrijving</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>Academische bibliografie UHasselt</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\URL Type\</t>
+  </si>
+  <si>
+    <t>Agrippa</t>
+  </si>
+  <si>
+    <t>Bibliotheekcollectie in EHC</t>
+  </si>
+  <si>
+    <t>DAMS Archief</t>
+  </si>
+  <si>
+    <t>Erfgoedbibliotheek Hendrik Conscience, Antwerpen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FelixArchief Antwerpen </t>
+  </si>
+  <si>
+    <t>Google Books</t>
+  </si>
+  <si>
+    <t>Verwijzing naar de archiefbeschrijvingen bij LH</t>
+  </si>
+  <si>
+    <t>Verwijzing naar de archiefbeschrijvingen bij MPM</t>
+  </si>
+  <si>
+    <t>Verwijzing naar de archiefbeschrijvingen bij RUB</t>
+  </si>
+  <si>
+    <t>Link naar record in search.museumplantinmoretus.be</t>
+  </si>
+  <si>
+    <t>Verwijzing naar LH objectbeschrijvingen</t>
+  </si>
+  <si>
+    <t>Verwijzing naar MPM objectbeschrijvingen</t>
+  </si>
+  <si>
+    <t>Verwijzing naar Grossmann object</t>
+  </si>
+  <si>
+    <t>Publicaties in de Anet catalogus</t>
+  </si>
+  <si>
+    <t>Link naar bibliotheekcatalogus EHC</t>
+  </si>
+  <si>
+    <t>zie verder bibliotheekcatalogus Museum Plantin Moretus</t>
+  </si>
+  <si>
+    <t>Bibliotheekcatalogus van het Rubenianum</t>
+  </si>
+  <si>
+    <t>PURL</t>
+  </si>
+  <si>
+    <t>RKDimages</t>
+  </si>
+  <si>
+    <t>Publicaties in de STCV catalogus</t>
+  </si>
+  <si>
+    <t>uniform resource locators</t>
+  </si>
+  <si>
+    <t>WorldCat</t>
+  </si>
+  <si>
+    <t>Wikipedia (DE)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -417,12 +506,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -438,16 +533,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -463,7 +559,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="date_types" connectionId="1" xr16:uid="{BB098E16-91BC-9844-9634-C6D74AF61275}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="date_types" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -762,36 +858,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA66850A-322F-E444-9A49-A75179311733}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.296875" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -802,16 +907,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7647E7-4FB2-D64B-A5A6-0453F042239A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -820,46 +925,58 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8D8E59-F71A-C140-A041-A98645C980AD}">
-  <dimension ref="B1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -868,18 +985,18 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD6203A-12C1-F24F-81E1-6F53C98FF933}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -888,213 +1005,423 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A78AFF1-203A-0244-8E33-66670FC8C342}">
-  <dimension ref="A1:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="27.8984375" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="C15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="C21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="C22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="C23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E23">
+        <v>300404630</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="C24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51A7DFE-1560-E441-9194-CA9CBD226C47}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.69921875" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3">
+        <v>300435416</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="F5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="F6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1103,21 +1430,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760649D4-A380-BA45-993D-A5C55AF90162}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1126,101 +1453,110 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E941267-4D9C-494F-987C-2EFFE548C7F3}">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1229,16 +1565,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B61536-1D9C-AF45-A302-E3A6FE8A0804}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1247,82 +1583,91 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1B2AC8-095A-BB47-B1E8-F73316A93EA1}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.796875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1331,18 +1676,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A39811-3E68-BC47-B72D-0D36849595BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1351,69 +1696,81 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFFFB3D-6997-744D-9C09-114AA1E73CEA}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1422,23 +1779,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78713D42-5181-AA45-82B9-E4381AAD1FA0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1447,107 +1804,116 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A66FFD1-A8DD-5244-9B58-A10E4BFA9F2D}">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correspondence Type Measurement Units Identifier Type
</commit_message>
<xml_diff>
--- a/admin/rdm/Digiplois_RDM_not_ObjK.xlsx
+++ b/admin/rdm/Digiplois_RDM_not_ObjK.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1176" yWindow="1464" windowWidth="27240" windowHeight="16044" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="1176" yWindow="1464" windowWidth="27240" windowHeight="16044"/>
   </bookViews>
   <sheets>
     <sheet name="Correspondence Type" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="162">
   <si>
     <t>code</t>
   </si>
@@ -467,6 +467,87 @@
   </si>
   <si>
     <t>Wikipedia (DE)</t>
+  </si>
+  <si>
+    <t>aanwinst identifier</t>
+  </si>
+  <si>
+    <t>archief identifier</t>
+  </si>
+  <si>
+    <t>accession numbers</t>
+  </si>
+  <si>
+    <t>bewaarinstelling identifier</t>
+  </si>
+  <si>
+    <t>shelf marks</t>
+  </si>
+  <si>
+    <t>object identifier</t>
+  </si>
+  <si>
+    <t>repository numbers</t>
+  </si>
+  <si>
+    <t>call numbers</t>
+  </si>
+  <si>
+    <t>record identifiers</t>
+  </si>
+  <si>
+    <t>referentienummer</t>
+  </si>
+  <si>
+    <t>aanwinst nummer</t>
+  </si>
+  <si>
+    <t>archief nummer</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Identifier Type\</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Meeteenheid Type\</t>
+  </si>
+  <si>
+    <t>millimeters</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>centimeters</t>
+  </si>
+  <si>
+    <t>pages (components)</t>
+  </si>
+  <si>
+    <t>pagina</t>
+  </si>
+  <si>
+    <t>folio</t>
+  </si>
+  <si>
+    <t>folios (leaves)</t>
+  </si>
+  <si>
+    <t>vel</t>
+  </si>
+  <si>
+    <t>sheets (paper artifacts)</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\ISAAR Relatie Type\</t>
+  </si>
+  <si>
+    <t>recipients (people)</t>
+  </si>
+  <si>
+    <t>correspondents (correspondence writers)</t>
   </si>
 </sst>
 </file>
@@ -861,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -895,10 +976,28 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2">
+        <v>300443565</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3">
+        <v>300225705</v>
       </c>
     </row>
   </sheetData>
@@ -1011,9 +1110,9 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomLeft" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1339,7 +1438,7 @@
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="35.69921875" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="34.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1431,6 +1530,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1780,40 +1882,142 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A4"/>
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="34.796875" customWidth="1"/>
+    <col min="4" max="4" width="19.69921875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2">
+        <v>300379097</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3">
+        <v>300379098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4">
+        <v>300194222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5">
+        <v>300189604</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6">
+        <v>300189648</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="32.69921875" customWidth="1"/>
+    <col min="3" max="3" width="34.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1840,83 +2044,204 @@
       <c r="B2" t="s">
         <v>47</v>
       </c>
+      <c r="C2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>47</v>
       </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>50</v>
       </c>
+      <c r="C5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>48</v>
       </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>51</v>
       </c>
+      <c r="C7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7">
+        <v>300312355</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>52</v>
       </c>
+      <c r="C8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>53</v>
       </c>
+      <c r="C9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9">
+        <v>300404704</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>54</v>
       </c>
+      <c r="C10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>55</v>
       </c>
+      <c r="C11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11">
+        <v>300404621</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>56</v>
       </c>
+      <c r="C12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12">
+        <v>300311706</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>57</v>
       </c>
+      <c r="C13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13">
+        <v>300435704</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>58</v>
       </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14">
+        <v>300435704</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>59</v>
       </c>
+      <c r="C15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16">
+        <v>300404630</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>61</v>
       </c>
+      <c r="C17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17">
+        <v>300311706</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>